<commit_message>
added calculator with st.form
</commit_message>
<xml_diff>
--- a/Extracted_phys_exam-updated4.23.25.xlsx
+++ b/Extracted_phys_exam-updated4.23.25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/courtneyreamer/Documents/GitHub/BedsideDx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{26F0F2F5-98C0-4B40-8A95-7DCD56C9ACFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C976D76-2B93-2645-995E-1520ACB63368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{DB31A4BA-DEDC-0F45-BC36-F69C9984D489}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="207">
   <si>
     <t>Physical exam maneuver</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Arterial pulse palpation</t>
   </si>
   <si>
-    <t>Delayed carotid artery upstroke5,9–13</t>
-  </si>
-  <si>
     <t>31–91</t>
   </si>
   <si>
@@ -100,24 +97,12 @@
     <t>65–81</t>
   </si>
   <si>
-    <t>Brachioradial delay14</t>
-  </si>
-  <si>
     <t>Apical impulse</t>
   </si>
   <si>
-    <t>Sustained apical impulse10</t>
-  </si>
-  <si>
-    <t>Apical-carotid delay15</t>
-  </si>
-  <si>
     <t>cardiac auscultation</t>
   </si>
   <si>
-    <t>Absent or diminished S5,9,11–13,16</t>
-  </si>
-  <si>
     <t>44–90</t>
   </si>
   <si>
@@ -136,9 +121,6 @@
     <t>NS</t>
   </si>
   <si>
-    <t>aortic systolic murmur oudest over aortic area11,12</t>
-  </si>
-  <si>
     <t>58–75</t>
   </si>
   <si>
@@ -148,18 +130,12 @@
     <t>Murmur</t>
   </si>
   <si>
-    <t>aortic systolic mumur with radiation to neck5,11–13</t>
-  </si>
-  <si>
     <t>90–98</t>
   </si>
   <si>
     <t>11–51</t>
   </si>
   <si>
-    <t>aortic systolic murmur with radiation to both sides of neck5</t>
-  </si>
-  <si>
     <t>skin inspection</t>
   </si>
   <si>
@@ -175,39 +151,24 @@
     <t xml:space="preserve">pallor </t>
   </si>
   <si>
-    <t>Nailbed pallor4,5,8</t>
-  </si>
-  <si>
     <t>41–60</t>
   </si>
   <si>
     <t>66–93</t>
   </si>
   <si>
-    <t>Palmar pallor4,5</t>
-  </si>
-  <si>
     <t>58–64</t>
   </si>
   <si>
     <t>74–96</t>
   </si>
   <si>
-    <t>Palmar crease pallor4</t>
-  </si>
-  <si>
-    <t>Conjunctival pallor4,5,10,11</t>
-  </si>
-  <si>
     <t>31–62</t>
   </si>
   <si>
     <t>82–97</t>
   </si>
   <si>
-    <t>Tongue pallor12</t>
-  </si>
-  <si>
     <t>conjunctiva inspection</t>
   </si>
   <si>
@@ -241,12 +202,6 @@
     <t>aortic regurgitation, detecting dilated aortic root</t>
   </si>
   <si>
-    <t>endocarditis3"""</t>
-  </si>
-  <si>
-    <t>diastolic murmur grade 3 or louder41,51</t>
-  </si>
-  <si>
     <t>30–61</t>
   </si>
   <si>
@@ -271,15 +226,6 @@
     <t>hill test</t>
   </si>
   <si>
-    <t>Foot-arm systolic blood pressure difference &gt;</t>
-  </si>
-  <si>
-    <t>40 mm Hg52</t>
-  </si>
-  <si>
-    <t>53"</t>
-  </si>
-  <si>
     <t>45–70</t>
   </si>
   <si>
@@ -316,60 +262,36 @@
     <t>body habitus inspection</t>
   </si>
   <si>
-    <t>Moon faciesf6</t>
-  </si>
-  <si>
     <t>cushing's syndrome</t>
   </si>
   <si>
     <t>Body habitus</t>
   </si>
   <si>
-    <t>Dorsal cervical fat pad45</t>
-  </si>
-  <si>
-    <t>Thin skinfold15</t>
-  </si>
-  <si>
     <t>Skin findings</t>
   </si>
   <si>
-    <t>Plethora5</t>
-  </si>
-  <si>
     <t>inspection</t>
   </si>
   <si>
-    <t>Hirsutism, in women5,6,30,45</t>
-  </si>
-  <si>
     <t>31–76</t>
   </si>
   <si>
     <t>48–79</t>
   </si>
   <si>
-    <t>Ecchymoses5,6,30</t>
-  </si>
-  <si>
     <t>38–71</t>
   </si>
   <si>
     <t>69–94</t>
   </si>
   <si>
-    <t>Red or blue striae5,6,30,45</t>
-  </si>
-  <si>
     <t>15–52</t>
   </si>
   <si>
     <t>61–93</t>
   </si>
   <si>
-    <t>Acne5,30</t>
-  </si>
-  <si>
     <t>25–52</t>
   </si>
   <si>
@@ -379,9 +301,6 @@
     <t>extremity strength exam</t>
   </si>
   <si>
-    <t>Muscle weakness5,6,30,45</t>
-  </si>
-  <si>
     <t>28–63</t>
   </si>
   <si>
@@ -394,9 +313,6 @@
     <t>extremity examination</t>
   </si>
   <si>
-    <t>Edema5,6</t>
-  </si>
-  <si>
     <t>38–57</t>
   </si>
   <si>
@@ -406,24 +322,15 @@
     <t>lung examination</t>
   </si>
   <si>
-    <t>Asymmetric chest expansion3</t>
-  </si>
-  <si>
     <t>pneumonia</t>
   </si>
   <si>
     <t>lung findings</t>
   </si>
   <si>
-    <t>Chest wall tenderness15</t>
-  </si>
-  <si>
     <t>percustion of lungs</t>
   </si>
   <si>
-    <t>Percussion dullness3–5,20–23</t>
-  </si>
-  <si>
     <t>4–26</t>
   </si>
   <si>
@@ -433,15 +340,6 @@
     <t>ausculation of lungs</t>
   </si>
   <si>
-    <t>Diminished breath</t>
-  </si>
-  <si>
-    <t>sounds</t>
-  </si>
-  <si>
-    <t>Bronchial breath sounds4,22</t>
-  </si>
-  <si>
     <t>14–19</t>
   </si>
   <si>
@@ -451,27 +349,18 @@
     <t>egophony</t>
   </si>
   <si>
-    <t>Egophony3–5</t>
-  </si>
-  <si>
     <t>4–16</t>
   </si>
   <si>
     <t>96–99</t>
   </si>
   <si>
-    <t>Crackles3–6,9,10,13–15,20,21,24</t>
-  </si>
-  <si>
     <t>19–67</t>
   </si>
   <si>
     <t>36–97</t>
   </si>
   <si>
-    <t>Wheezing4–6,9,13,15,20,21,24</t>
-  </si>
-  <si>
     <t>4–36</t>
   </si>
   <si>
@@ -481,33 +370,15 @@
     <t>chest examination</t>
   </si>
   <si>
-    <t>Barrel chest11</t>
-  </si>
-  <si>
     <t>copd</t>
   </si>
   <si>
-    <t>AP/L chest diameter ratio ≥0.911</t>
-  </si>
-  <si>
-    <t>Pursed-lip breathing11</t>
-  </si>
-  <si>
     <t>inspection for respiratory distress</t>
   </si>
   <si>
-    <t>Scalene/sternocleidomastoid muscle use11</t>
-  </si>
-  <si>
     <t>laryngeal height measurement</t>
   </si>
   <si>
-    <t>Maximum laryngeal height ≤4 cm12</t>
-  </si>
-  <si>
-    <t>Hoover sign13</t>
-  </si>
-  <si>
     <t>precordial palpation</t>
   </si>
   <si>
@@ -523,39 +394,24 @@
     <t>chest percussion</t>
   </si>
   <si>
-    <t>Absent cardiac dullness left lower sternal</t>
-  </si>
-  <si>
-    <t>border5"</t>
-  </si>
-  <si>
     <t>Percussion of lungs</t>
   </si>
   <si>
     <t>lung percussion</t>
   </si>
   <si>
-    <t>Hyperresonance of chest5,14</t>
-  </si>
-  <si>
     <t>21–33</t>
   </si>
   <si>
     <t>94–98</t>
   </si>
   <si>
-    <t>Diaphragm excursion percussed &lt;2 cm5</t>
-  </si>
-  <si>
     <t>percussino of lungs</t>
   </si>
   <si>
     <t>lung auscultation</t>
   </si>
   <si>
-    <t>Reduced breath sounds5,11,13–15</t>
-  </si>
-  <si>
     <t>29–82</t>
   </si>
   <si>
@@ -565,18 +421,12 @@
     <t>auscultation of lungs</t>
   </si>
   <si>
-    <t>Early inspiratory crackles18,19</t>
-  </si>
-  <si>
     <t>25–77</t>
   </si>
   <si>
     <t>97–98</t>
   </si>
   <si>
-    <t>Any unforced wheeze5,6,12–14,20,21</t>
-  </si>
-  <si>
     <t>13–56</t>
   </si>
   <si>
@@ -601,9 +451,6 @@
     <t>42–94</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>Forced expiratory time &lt;3 seconds</t>
   </si>
   <si>
@@ -652,9 +499,6 @@
     <t>https://physicaldiagnosispdx.com/endocrinology-multimedia/abdominal-striae/</t>
   </si>
   <si>
-    <t>s4 gallop</t>
-  </si>
-  <si>
     <t>https://physicaldiagnosispdx.com/cardiology-multimedia-new/s4-gallop/</t>
   </si>
   <si>
@@ -662,6 +506,141 @@
   </si>
   <si>
     <t>https://physicaldiagnosispdx.com/cardiology-multimedia-new/s3-gallop/</t>
+  </si>
+  <si>
+    <t>Delayed carotid artery upstroke</t>
+  </si>
+  <si>
+    <t>Brachioradial delay</t>
+  </si>
+  <si>
+    <t>Sustained apical impulse</t>
+  </si>
+  <si>
+    <t>Apical-carotid delay</t>
+  </si>
+  <si>
+    <t>Absent or diminished S2</t>
+  </si>
+  <si>
+    <t>S4 gallop</t>
+  </si>
+  <si>
+    <t>aortic systolic murmur oudest over aortic area</t>
+  </si>
+  <si>
+    <t>aortic systolic mumur with radiation to neck</t>
+  </si>
+  <si>
+    <t>aortic systolic murmur with radiation to both sides of neck</t>
+  </si>
+  <si>
+    <t>Nailbed pallor</t>
+  </si>
+  <si>
+    <t>Palmar pallor</t>
+  </si>
+  <si>
+    <t>Palmar crease pallor</t>
+  </si>
+  <si>
+    <t>Conjunctival pallor</t>
+  </si>
+  <si>
+    <t>Tongue pallor</t>
+  </si>
+  <si>
+    <t>diastolic murmur grade 3 or louder</t>
+  </si>
+  <si>
+    <t>Foot-arm systolic blood pressure difference &gt; 40</t>
+  </si>
+  <si>
+    <t>Moon faciesf</t>
+  </si>
+  <si>
+    <t>Dorsal cervical fat pad</t>
+  </si>
+  <si>
+    <t>Thin skinfold</t>
+  </si>
+  <si>
+    <t>Plethora</t>
+  </si>
+  <si>
+    <t>Hirsutism, in women5</t>
+  </si>
+  <si>
+    <t>Ecchymoses</t>
+  </si>
+  <si>
+    <t>Red or blue striae</t>
+  </si>
+  <si>
+    <t>Acne</t>
+  </si>
+  <si>
+    <t>Muscle weakness</t>
+  </si>
+  <si>
+    <t>Edema</t>
+  </si>
+  <si>
+    <t>Asymmetric chest expansion</t>
+  </si>
+  <si>
+    <t>Chest wall tenderness</t>
+  </si>
+  <si>
+    <t>Percussion dullness</t>
+  </si>
+  <si>
+    <t>Bronchial breath sounds</t>
+  </si>
+  <si>
+    <t>Egophony</t>
+  </si>
+  <si>
+    <t>Crackles</t>
+  </si>
+  <si>
+    <t>Wheezing</t>
+  </si>
+  <si>
+    <t>Barrel chest</t>
+  </si>
+  <si>
+    <t>AP/L chest diameter ratio ≥0.9</t>
+  </si>
+  <si>
+    <t>Pursed-lip breathing</t>
+  </si>
+  <si>
+    <t>Scalene/sternocleidomastoid muscle use</t>
+  </si>
+  <si>
+    <t>Maximum laryngeal height ≤4 cm</t>
+  </si>
+  <si>
+    <t>Hoover sign</t>
+  </si>
+  <si>
+    <t>Absent cardiac dullness left lower sternal border</t>
+  </si>
+  <si>
+    <t>Hyperresonance of chest</t>
+  </si>
+  <si>
+    <t>Diaphragm excursion percussed &lt;2 cm</t>
+  </si>
+  <si>
+    <t>Reduced breath sounds</t>
+  </si>
+  <si>
+    <t>Early inspiratory crackles</t>
+  </si>
+  <si>
+    <t>Any unforced wheeze</t>
   </si>
 </sst>
 </file>
@@ -1522,10 +1501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BDB451C-1826-564E-B434-A7A374458D44}">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1566,10 +1545,10 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
-        <v>198</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1604,7 +1583,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1612,13 +1591,13 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
       </c>
       <c r="E3">
         <v>3.5</v>
@@ -1627,13 +1606,13 @@
         <v>0.4</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -1644,13 +1623,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
       <c r="E4">
         <v>2.2999999999999998</v>
@@ -1659,13 +1638,13 @@
         <v>0.4</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J4">
         <v>5</v>
@@ -1676,7 +1655,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>163</v>
       </c>
       <c r="C5">
         <v>97</v>
@@ -1691,13 +1670,13 @@
         <v>0.04</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J5">
         <v>5</v>
@@ -1705,10 +1684,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>164</v>
       </c>
       <c r="C6">
         <v>78</v>
@@ -1723,13 +1702,13 @@
         <v>0.3</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -1737,10 +1716,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="C7">
         <v>97</v>
@@ -1755,13 +1734,13 @@
         <v>0.05</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J7">
         <v>5</v>
@@ -1769,16 +1748,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>3.8</v>
@@ -1787,13 +1766,13 @@
         <v>0.4</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="J8">
         <v>5</v>
@@ -1801,179 +1780,203 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="B9">
-        <v>2</v>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>210</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>1.8</v>
+      </c>
+      <c r="F10">
+        <v>0.6</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J10">
         <v>5</v>
       </c>
       <c r="K10" t="s">
-        <v>211</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="F11">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" t="s">
         <v>15</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J11">
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
+        <v>170</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>74</v>
       </c>
       <c r="E12">
-        <v>1.4</v>
-      </c>
-      <c r="F12">
-        <v>0.1</v>
+        <v>1.9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
         <v>15</v>
       </c>
       <c r="I12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="J12">
         <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>200</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C13">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="E13">
-        <v>1.9</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
+        <v>3.8</v>
+      </c>
+      <c r="F13">
+        <v>0.6</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13" t="s">
-        <v>200</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14">
-        <v>46</v>
-      </c>
-      <c r="D14">
-        <v>88</v>
+        <v>171</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
       </c>
       <c r="E14">
-        <v>3.8</v>
+        <v>4.3</v>
       </c>
       <c r="F14">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J14">
         <v>5.6</v>
@@ -1981,699 +1984,753 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
-      </c>
       <c r="E15">
-        <v>4.3</v>
+        <v>5.6</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J15">
         <v>5.6</v>
       </c>
+      <c r="L15" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
+        <v>173</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>99</v>
       </c>
       <c r="E16">
-        <v>5.6</v>
-      </c>
-      <c r="F16">
-        <v>0.4</v>
+        <v>7.9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I16" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J16">
         <v>5.6</v>
       </c>
-      <c r="L16" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17">
-        <v>8</v>
-      </c>
-      <c r="D17">
-        <v>99</v>
+        <v>174</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
       </c>
       <c r="E17">
-        <v>7.9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
+        <v>4.7</v>
+      </c>
+      <c r="F17">
+        <v>0.6</v>
       </c>
       <c r="G17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J17">
         <v>5.6</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
+        <v>175</v>
+      </c>
+      <c r="C18">
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <v>87</v>
       </c>
       <c r="E18">
-        <v>4.7</v>
+        <v>3.7</v>
       </c>
       <c r="F18">
         <v>0.6</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="J18">
         <v>5.6</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C19">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="D19">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E19">
-        <v>3.7</v>
-      </c>
-      <c r="F19">
-        <v>0.6</v>
+        <v>16.7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J19">
         <v>5.6</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20">
-        <v>10</v>
-      </c>
-      <c r="D20">
-        <v>99</v>
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
       </c>
       <c r="E20">
-        <v>16.7</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
+        <v>10.1</v>
+      </c>
+      <c r="F20">
+        <v>0.3</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="J20">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" t="s">
-        <v>68</v>
+        <v>58</v>
+      </c>
+      <c r="C21">
+        <v>29</v>
+      </c>
+      <c r="D21">
+        <v>96</v>
       </c>
       <c r="E21">
-        <v>10.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F21">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="J21">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22">
-        <v>29</v>
-      </c>
-      <c r="D22">
-        <v>96</v>
+        <v>176</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
       </c>
       <c r="E22">
         <v>8.1999999999999993</v>
       </c>
       <c r="F22">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="H22" t="s">
-        <v>72</v>
+        <v>56</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
       </c>
       <c r="J22">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>57</v>
+      </c>
+      <c r="D23">
+        <v>95</v>
+      </c>
+      <c r="E23">
+        <v>10.9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>177</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E24">
-        <v>8.1999999999999993</v>
+        <v>6</v>
       </c>
       <c r="F24">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J24">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C25">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D25">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="E25">
-        <v>10.9</v>
-      </c>
-      <c r="F25" t="s">
-        <v>48</v>
+        <v>2.4</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="I25" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J25">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>97</v>
+      </c>
+      <c r="E26">
+        <v>5.9</v>
+      </c>
+      <c r="F26">
+        <v>0.8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K26" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>40</v>
       </c>
       <c r="F27">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H27" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="I27" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="J27">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28">
-        <v>52</v>
-      </c>
-      <c r="D28">
-        <v>60</v>
-      </c>
-      <c r="E28">
-        <v>2.4</v>
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
       </c>
       <c r="F28">
-        <v>0.1</v>
+        <v>0.7</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="I28" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="J28">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>212</v>
-      </c>
-      <c r="C29">
-        <v>20</v>
-      </c>
-      <c r="D29">
-        <v>97</v>
-      </c>
-      <c r="E29">
-        <v>5.9</v>
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
       </c>
       <c r="F29">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G29" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="I29" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="J29">
         <v>4.9000000000000004</v>
       </c>
-      <c r="K29" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>48</v>
+        <v>178</v>
+      </c>
+      <c r="C30">
+        <v>98</v>
+      </c>
+      <c r="D30">
+        <v>41</v>
+      </c>
+      <c r="E30">
+        <v>1.6</v>
       </c>
       <c r="F30">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="G30" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="I30" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J30">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="L30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" t="s">
-        <v>37</v>
+        <v>179</v>
+      </c>
+      <c r="C31">
+        <v>50</v>
+      </c>
+      <c r="D31">
+        <v>78</v>
+      </c>
+      <c r="E31">
+        <v>2.2999999999999998</v>
       </c>
       <c r="F31">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="G31" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="H31" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="I31" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="J31">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="L31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" t="s">
-        <v>37</v>
+        <v>180</v>
+      </c>
+      <c r="C32">
+        <v>78</v>
+      </c>
+      <c r="D32">
+        <v>99</v>
+      </c>
+      <c r="E32">
+        <v>115.6</v>
       </c>
       <c r="F32">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="H32" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="I32" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J32">
-        <v>4.9000000000000004</v>
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="L32" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>181</v>
       </c>
       <c r="C33">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D33">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="E33">
-        <v>1.6</v>
+        <v>2.7</v>
       </c>
       <c r="F33">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="G33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H33" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I33" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="J33">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="L33" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34">
-        <v>50</v>
-      </c>
-      <c r="D34">
-        <v>78</v>
+        <v>182</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>85</v>
       </c>
       <c r="E34">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="F34">
-        <v>0.6</v>
+        <v>1.4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
       </c>
       <c r="G34" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H34" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I34" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="J34">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="L34" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35">
-        <v>78</v>
-      </c>
-      <c r="D35">
-        <v>99</v>
+        <v>183</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
+        <v>87</v>
       </c>
       <c r="E35">
-        <v>115.6</v>
+        <v>4.5</v>
       </c>
       <c r="F35">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="G35" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H35" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I35" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="J35">
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="L35" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36">
-        <v>83</v>
-      </c>
-      <c r="D36">
-        <v>69</v>
+        <v>184</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>89</v>
       </c>
       <c r="E36">
-        <v>2.7</v>
-      </c>
-      <c r="F36">
-        <v>0.3</v>
+        <v>1.7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>32</v>
       </c>
       <c r="G36" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H36" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I36" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="J36">
         <v>6.7999999999999996E-3</v>
       </c>
+      <c r="L36" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D37" t="s">
-        <v>108</v>
-      </c>
-      <c r="E37">
-        <v>1.4</v>
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
+        <v>32</v>
       </c>
       <c r="F37" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G37" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H37" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I37" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="J37">
         <v>6.7999999999999996E-3</v>
@@ -2681,446 +2738,491 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>109</v>
+        <v>186</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="E38">
-        <v>4.5</v>
-      </c>
-      <c r="F38">
-        <v>0.6</v>
+        <v>3.8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
       </c>
       <c r="G38" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H38" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I38" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J38">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="L38" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>187</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="E39">
-        <v>1.7</v>
-      </c>
-      <c r="F39" t="s">
-        <v>37</v>
+        <v>1.8</v>
+      </c>
+      <c r="F39">
+        <v>0.7</v>
       </c>
       <c r="G39" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H39" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="I39" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="J39">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="L39" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" t="s">
-        <v>37</v>
+        <v>188</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>100</v>
+      </c>
+      <c r="E40">
+        <v>44.1</v>
       </c>
       <c r="F40" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G40" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H40" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J40">
-        <v>6.7999999999999996E-3</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" t="s">
-        <v>121</v>
-      </c>
-      <c r="E41">
-        <v>3.8</v>
+        <v>189</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>96</v>
+      </c>
+      <c r="E41" t="s">
+        <v>32</v>
       </c>
       <c r="F41" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G41" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I41" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="J41">
-        <v>6.7999999999999996E-3</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D42" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E42">
-        <v>1.8</v>
-      </c>
-      <c r="F42">
-        <v>0.7</v>
+        <v>3.6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
       </c>
       <c r="G42" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H42" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I42" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="J42">
-        <v>6.7999999999999996E-3</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43">
-        <v>5</v>
-      </c>
-      <c r="D43">
+        <v>191</v>
+      </c>
+      <c r="C43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43">
+        <v>3.3</v>
+      </c>
+      <c r="F43">
+        <v>0.9</v>
+      </c>
+      <c r="G43" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" t="s">
         <v>100</v>
       </c>
-      <c r="E43">
-        <v>44.1</v>
-      </c>
-      <c r="F43" t="s">
-        <v>37</v>
-      </c>
-      <c r="G43" t="s">
-        <v>48</v>
-      </c>
-      <c r="H43" t="s">
-        <v>129</v>
-      </c>
       <c r="I43" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="J43">
         <v>2.48</v>
       </c>
+      <c r="K43" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
-      </c>
-      <c r="C44">
-        <v>5</v>
-      </c>
-      <c r="D44">
-        <v>96</v>
-      </c>
-      <c r="E44" t="s">
-        <v>37</v>
+        <v>192</v>
+      </c>
+      <c r="C44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44">
+        <v>4.0999999999999996</v>
       </c>
       <c r="F44" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G44" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H44" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="I44" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="J44">
         <v>2.48</v>
       </c>
+      <c r="K44" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>193</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="E45">
-        <v>3.6</v>
-      </c>
-      <c r="F45" t="s">
-        <v>37</v>
+        <v>2.8</v>
+      </c>
+      <c r="F45">
+        <v>0.8</v>
       </c>
       <c r="G45" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H45" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="I45" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="J45">
         <v>2.48</v>
       </c>
+      <c r="K45" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>194</v>
+      </c>
+      <c r="C46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46">
+        <v>0.8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" t="s">
+        <v>40</v>
+      </c>
+      <c r="H46" t="s">
+        <v>100</v>
+      </c>
+      <c r="I46" t="s">
+        <v>101</v>
+      </c>
+      <c r="J46">
+        <v>2.48</v>
+      </c>
+      <c r="K46" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>115</v>
+      </c>
+      <c r="B47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47">
+        <v>65</v>
+      </c>
+      <c r="D47">
+        <v>58</v>
+      </c>
+      <c r="E47">
+        <v>1.5</v>
+      </c>
+      <c r="F47">
+        <v>0.6</v>
+      </c>
+      <c r="G47" t="s">
+        <v>40</v>
+      </c>
+      <c r="H47" t="s">
+        <v>116</v>
+      </c>
+      <c r="I47" t="s">
+        <v>40</v>
+      </c>
+      <c r="J47">
+        <v>6.5</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" t="s">
-        <v>140</v>
-      </c>
-      <c r="D48" t="s">
-        <v>141</v>
+        <v>196</v>
+      </c>
+      <c r="C48">
+        <v>31</v>
+      </c>
+      <c r="D48">
+        <v>84</v>
       </c>
       <c r="E48">
-        <v>3.3</v>
-      </c>
-      <c r="F48">
-        <v>0.9</v>
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
       </c>
       <c r="G48" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H48" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I48" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="J48">
-        <v>2.48</v>
-      </c>
-      <c r="K48" t="s">
-        <v>204</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" t="s">
-        <v>144</v>
-      </c>
-      <c r="D49" t="s">
-        <v>145</v>
+        <v>197</v>
+      </c>
+      <c r="C49">
+        <v>58</v>
+      </c>
+      <c r="D49">
+        <v>78</v>
       </c>
       <c r="E49">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F49" t="s">
-        <v>37</v>
+        <v>2.7</v>
+      </c>
+      <c r="F49">
+        <v>0.5</v>
       </c>
       <c r="G49" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H49" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I49" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="J49">
-        <v>2.48</v>
-      </c>
-      <c r="K49" t="s">
-        <v>203</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
-      </c>
-      <c r="C50" t="s">
-        <v>147</v>
-      </c>
-      <c r="D50" t="s">
-        <v>148</v>
+        <v>198</v>
+      </c>
+      <c r="C50">
+        <v>39</v>
+      </c>
+      <c r="D50">
+        <v>88</v>
       </c>
       <c r="E50">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
       <c r="F50">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G50" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H50" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I50" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="J50">
-        <v>2.48</v>
-      </c>
-      <c r="K50" t="s">
-        <v>201</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" t="s">
-        <v>150</v>
-      </c>
-      <c r="D51" t="s">
-        <v>151</v>
+        <v>199</v>
+      </c>
+      <c r="C51">
+        <v>36</v>
+      </c>
+      <c r="D51">
+        <v>90</v>
       </c>
       <c r="E51">
-        <v>0.8</v>
-      </c>
-      <c r="F51" t="s">
-        <v>37</v>
+        <v>3.6</v>
+      </c>
+      <c r="F51">
+        <v>0.7</v>
       </c>
       <c r="G51" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H51" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="I51" t="s">
-        <v>130</v>
+        <v>40</v>
       </c>
       <c r="J51">
-        <v>2.48</v>
-      </c>
-      <c r="K51" t="s">
-        <v>202</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="B52" t="s">
-        <v>153</v>
+        <v>200</v>
       </c>
       <c r="C52">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D52">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="E52">
-        <v>1.5</v>
+        <v>4.2</v>
       </c>
       <c r="F52">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="G52" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H52" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I52" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J52">
         <v>6.5</v>
@@ -3128,31 +3230,31 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
-      </c>
-      <c r="C53">
-        <v>31</v>
-      </c>
-      <c r="D53">
-        <v>84</v>
+        <v>120</v>
+      </c>
+      <c r="C53" t="s">
+        <v>121</v>
+      </c>
+      <c r="D53" t="s">
+        <v>122</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>7.4</v>
       </c>
       <c r="F53" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G53" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H53" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I53" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="J53">
         <v>6.5</v>
@@ -3160,31 +3262,31 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>201</v>
       </c>
       <c r="C54">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="D54">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="E54">
-        <v>2.7</v>
-      </c>
-      <c r="F54">
-        <v>0.5</v>
+        <v>11.8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>32</v>
       </c>
       <c r="G54" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H54" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I54" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="J54">
         <v>6.5</v>
@@ -3192,31 +3294,31 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>158</v>
-      </c>
-      <c r="C55">
-        <v>39</v>
-      </c>
-      <c r="D55">
-        <v>88</v>
+        <v>202</v>
+      </c>
+      <c r="C55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" t="s">
+        <v>127</v>
       </c>
       <c r="E55">
-        <v>3.3</v>
+        <v>7.3</v>
       </c>
       <c r="F55">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G55" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H55" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I55" t="s">
-        <v>48</v>
+        <v>124</v>
       </c>
       <c r="J55">
         <v>6.5</v>
@@ -3224,31 +3326,31 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="C56">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D56">
-        <v>90</v>
-      </c>
-      <c r="E56">
-        <v>3.6</v>
-      </c>
-      <c r="F56">
-        <v>0.7</v>
+        <v>98</v>
+      </c>
+      <c r="E56" t="s">
+        <v>32</v>
+      </c>
+      <c r="F56" t="s">
+        <v>32</v>
       </c>
       <c r="G56" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H56" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I56" t="s">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="J56">
         <v>6.5</v>
@@ -3256,31 +3358,31 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
-      </c>
-      <c r="C57">
-        <v>58</v>
-      </c>
-      <c r="D57">
-        <v>86</v>
+        <v>204</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" t="s">
+        <v>131</v>
       </c>
       <c r="E57">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="F57">
         <v>0.5</v>
       </c>
       <c r="G57" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H57" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I57" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="J57">
         <v>6.5</v>
@@ -3288,97 +3390,127 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>162</v>
+        <v>129</v>
       </c>
       <c r="B58" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C58" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="D58" t="s">
-        <v>165</v>
+        <v>134</v>
       </c>
       <c r="E58">
-        <v>7.4</v>
+        <v>14.6</v>
       </c>
       <c r="F58" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G58" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H58" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I58" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="J58">
         <v>6.5</v>
       </c>
+      <c r="K58" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>167</v>
+        <v>206</v>
+      </c>
+      <c r="C59" t="s">
+        <v>135</v>
+      </c>
+      <c r="D59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59">
+        <v>2.6</v>
+      </c>
+      <c r="F59">
+        <v>0.8</v>
+      </c>
+      <c r="G59" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" t="s">
+        <v>116</v>
+      </c>
+      <c r="I59" t="s">
+        <v>132</v>
+      </c>
+      <c r="J59">
+        <v>6.5</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>168</v>
-      </c>
-      <c r="B60">
-        <v>15</v>
-      </c>
-      <c r="C60">
-        <v>99</v>
-      </c>
-      <c r="D60">
-        <v>11.8</v>
-      </c>
-      <c r="E60" t="s">
-        <v>37</v>
+        <v>137</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60">
+        <v>3.9</v>
       </c>
       <c r="F60" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G60" t="s">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="H60" t="s">
-        <v>169</v>
+        <v>116</v>
+      </c>
+      <c r="I60" t="s">
+        <v>140</v>
+      </c>
+      <c r="J60">
+        <v>6.5</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="B61" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>172</v>
-      </c>
-      <c r="D61" t="s">
-        <v>173</v>
-      </c>
-      <c r="E61">
-        <v>7.3</v>
-      </c>
-      <c r="F61">
-        <v>0.8</v>
+        <v>142</v>
+      </c>
+      <c r="E61" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" t="s">
+        <v>40</v>
       </c>
       <c r="G61" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H61" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I61" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="J61">
         <v>6.5</v>
@@ -3386,228 +3518,33 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>174</v>
-      </c>
-      <c r="C62">
-        <v>13</v>
-      </c>
-      <c r="D62">
-        <v>98</v>
-      </c>
-      <c r="E62" t="s">
-        <v>37</v>
+        <v>143</v>
+      </c>
+      <c r="C62" t="s">
+        <v>144</v>
+      </c>
+      <c r="D62" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62">
+        <v>0.2</v>
       </c>
       <c r="F62" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G62" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="H62" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="I62" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="J62">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>176</v>
-      </c>
-      <c r="B63" t="s">
-        <v>177</v>
-      </c>
-      <c r="C63" t="s">
-        <v>178</v>
-      </c>
-      <c r="D63" t="s">
-        <v>179</v>
-      </c>
-      <c r="E63">
-        <v>3.5</v>
-      </c>
-      <c r="F63">
-        <v>0.5</v>
-      </c>
-      <c r="G63" t="s">
-        <v>48</v>
-      </c>
-      <c r="H63" t="s">
-        <v>154</v>
-      </c>
-      <c r="I63" t="s">
-        <v>180</v>
-      </c>
-      <c r="J63">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>176</v>
-      </c>
-      <c r="B64" t="s">
-        <v>181</v>
-      </c>
-      <c r="C64" t="s">
-        <v>182</v>
-      </c>
-      <c r="D64" t="s">
-        <v>183</v>
-      </c>
-      <c r="E64">
-        <v>14.6</v>
-      </c>
-      <c r="F64" t="s">
-        <v>37</v>
-      </c>
-      <c r="G64" t="s">
-        <v>48</v>
-      </c>
-      <c r="H64" t="s">
-        <v>154</v>
-      </c>
-      <c r="I64" t="s">
-        <v>180</v>
-      </c>
-      <c r="J64">
-        <v>6.5</v>
-      </c>
-      <c r="K64" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>176</v>
-      </c>
-      <c r="B65" t="s">
-        <v>184</v>
-      </c>
-      <c r="C65" t="s">
-        <v>185</v>
-      </c>
-      <c r="D65" t="s">
-        <v>186</v>
-      </c>
-      <c r="E65">
-        <v>2.6</v>
-      </c>
-      <c r="F65">
-        <v>0.8</v>
-      </c>
-      <c r="G65" t="s">
-        <v>48</v>
-      </c>
-      <c r="H65" t="s">
-        <v>154</v>
-      </c>
-      <c r="I65" t="s">
-        <v>180</v>
-      </c>
-      <c r="J65">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>187</v>
-      </c>
-      <c r="B66" t="s">
-        <v>188</v>
-      </c>
-      <c r="C66" t="s">
-        <v>189</v>
-      </c>
-      <c r="D66" t="s">
-        <v>186</v>
-      </c>
-      <c r="E66">
-        <v>3.9</v>
-      </c>
-      <c r="F66" t="s">
-        <v>48</v>
-      </c>
-      <c r="G66" t="s">
-        <v>48</v>
-      </c>
-      <c r="H66" t="s">
-        <v>154</v>
-      </c>
-      <c r="I66" t="s">
-        <v>190</v>
-      </c>
-      <c r="J66">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>187</v>
-      </c>
-      <c r="B67" t="s">
-        <v>191</v>
-      </c>
-      <c r="C67" t="s">
-        <v>192</v>
-      </c>
-      <c r="D67" t="s">
-        <v>193</v>
-      </c>
-      <c r="E67" t="s">
-        <v>37</v>
-      </c>
-      <c r="F67" t="s">
-        <v>48</v>
-      </c>
-      <c r="G67" t="s">
-        <v>48</v>
-      </c>
-      <c r="H67" t="s">
-        <v>154</v>
-      </c>
-      <c r="I67" t="s">
-        <v>190</v>
-      </c>
-      <c r="J67">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>187</v>
-      </c>
-      <c r="B68" t="s">
-        <v>194</v>
-      </c>
-      <c r="C68" t="s">
-        <v>195</v>
-      </c>
-      <c r="D68" t="s">
-        <v>196</v>
-      </c>
-      <c r="E68">
-        <v>0.2</v>
-      </c>
-      <c r="F68" t="s">
-        <v>48</v>
-      </c>
-      <c r="G68" t="s">
-        <v>48</v>
-      </c>
-      <c r="H68" t="s">
-        <v>154</v>
-      </c>
-      <c r="I68" t="s">
-        <v>190</v>
-      </c>
-      <c r="J68">
         <v>6.5</v>
       </c>
     </row>

</xml_diff>